<commit_message>
reviewing code for bugs
</commit_message>
<xml_diff>
--- a/CSV plan.xlsx
+++ b/CSV plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\nibrs_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7468A-51EC-4012-A217-1310D02DEFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DA8F75-5A93-40AF-9015-103BAF804A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E32AB67F-C50D-4B7B-BF96-2DF95897A32B}"/>
+    <workbookView xWindow="32100" yWindow="2310" windowWidth="14400" windowHeight="7815" xr2:uid="{E32AB67F-C50D-4B7B-BF96-2DF95897A32B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="127">
   <si>
     <t>Batch Header</t>
   </si>
@@ -263,12 +263,6 @@
     <t>primary_weapon_force</t>
   </si>
   <si>
-    <t>weapon_force_2</t>
-  </si>
-  <si>
-    <t>weapon_force_3</t>
-  </si>
-  <si>
     <t>Bias Motivation</t>
   </si>
   <si>
@@ -414,6 +408,12 @@
   </si>
   <si>
     <t>if "Y" True, "N" Flase elese:None</t>
+  </si>
+  <si>
+    <t>bias_group</t>
+  </si>
+  <si>
+    <t>✓</t>
   </si>
 </sst>
 </file>
@@ -819,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4CC23E-8A46-40A2-B7BE-F33F442EEB2C}">
-  <dimension ref="B2:J140"/>
+  <dimension ref="A2:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,12 +837,15 @@
     <col min="9" max="9" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -871,7 +874,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -900,7 +906,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -929,7 +938,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -958,7 +970,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -987,7 +1002,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1016,7 +1034,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -1045,7 +1066,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1074,7 +1098,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -1103,7 +1130,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1132,7 +1162,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
@@ -1152,7 +1185,7 @@
         <v>78</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>32</v>
@@ -1161,7 +1194,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
@@ -1190,7 +1226,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -1210,7 +1249,7 @@
         <v>96</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>33</v>
@@ -1219,7 +1258,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1242,7 +1284,7 @@
         <v>105, 114</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>35</v>
@@ -1251,12 +1293,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1285,7 +1330,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -1317,7 +1365,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1397,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -1379,12 +1433,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1413,7 +1470,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
       <c r="B26" t="s">
         <v>37</v>
       </c>
@@ -1445,7 +1505,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1474,7 +1537,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
       <c r="B28" t="s">
         <v>38</v>
       </c>
@@ -1507,12 +1573,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1541,7 +1610,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>126</v>
+      </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
@@ -1573,7 +1645,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>126</v>
+      </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -1602,7 +1677,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
@@ -1631,7 +1709,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>126</v>
+      </c>
       <c r="B36" t="s">
         <v>45</v>
       </c>
@@ -1660,7 +1741,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1689,7 +1773,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>126</v>
+      </c>
       <c r="B38" t="s">
         <v>45</v>
       </c>
@@ -1718,7 +1805,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>126</v>
+      </c>
       <c r="B39" t="s">
         <v>48</v>
       </c>
@@ -1741,7 +1831,7 @@
         <v>34, 36</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I39" t="s">
         <v>49</v>
@@ -1750,7 +1840,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>126</v>
+      </c>
       <c r="B40" t="s">
         <v>51</v>
       </c>
@@ -1782,7 +1875,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>126</v>
+      </c>
       <c r="B41" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1910,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
       <c r="B42" t="s">
         <v>57</v>
       </c>
@@ -1846,7 +1945,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>126</v>
+      </c>
       <c r="B43" t="s">
         <v>59</v>
       </c>
@@ -1878,7 +1980,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>126</v>
+      </c>
       <c r="B44" t="s">
         <v>62</v>
       </c>
@@ -1910,12 +2015,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>126</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
         <v>1</v>
       </c>
@@ -1944,7 +2052,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
       <c r="B48" t="s">
         <v>37</v>
       </c>
@@ -1976,7 +2087,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>126</v>
+      </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
@@ -2005,7 +2119,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>126</v>
+      </c>
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -2034,7 +2151,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
       <c r="B51" t="s">
         <v>45</v>
       </c>
@@ -2063,7 +2183,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
       <c r="B52" t="s">
         <v>45</v>
       </c>
@@ -2092,7 +2215,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
       <c r="B53" t="s">
         <v>45</v>
       </c>
@@ -2121,7 +2247,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>126</v>
+      </c>
       <c r="B54" t="s">
         <v>62</v>
       </c>
@@ -2153,7 +2282,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>126</v>
+      </c>
       <c r="B55" t="s">
         <v>67</v>
       </c>
@@ -2173,7 +2305,7 @@
         <v>36</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I55" t="s">
         <v>68</v>
@@ -2182,7 +2314,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>126</v>
+      </c>
       <c r="B56" t="s">
         <v>69</v>
       </c>
@@ -2214,7 +2349,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>126</v>
+      </c>
       <c r="B57" t="s">
         <v>71</v>
       </c>
@@ -2246,7 +2384,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>126</v>
+      </c>
       <c r="B58" t="s">
         <v>73</v>
       </c>
@@ -2262,7 +2403,7 @@
         <v>50</v>
       </c>
       <c r="H58" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I58" t="s">
         <v>74</v>
@@ -2271,1415 +2412,1490 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C59">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D59">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E59">
-        <f t="shared" ref="E59" si="22">C59-1</f>
-        <v>51</v>
+        <f t="shared" ref="E59:E60" si="22">C59-1</f>
+        <v>57</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59" si="23">D59</f>
-        <v>54</v>
+        <f t="shared" ref="F59:F60" si="23">D59</f>
+        <v>59</v>
       </c>
       <c r="G59" s="7" t="str">
-        <f t="shared" ref="G59" si="24">IF(D59 = 0, E59, _xlfn.CONCAT(E59, ", ", F59))</f>
-        <v>51, 54</v>
+        <f t="shared" ref="G59:G60" si="24">IF(D59 = 0, E59, _xlfn.CONCAT(E59, ", ", F59))</f>
+        <v>57, 59</v>
       </c>
       <c r="H59" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I59" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J59" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C60">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D60">
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="22"/>
         <v>57</v>
       </c>
-      <c r="E60">
-        <f t="shared" ref="E60:E62" si="25">C60-1</f>
-        <v>54</v>
-      </c>
       <c r="F60">
-        <f t="shared" ref="F60:F62" si="26">D60</f>
-        <v>57</v>
+        <f t="shared" si="23"/>
+        <v>59</v>
       </c>
       <c r="G60" s="7" t="str">
-        <f t="shared" ref="G60:G62" si="27">IF(D60 = 0, E60, _xlfn.CONCAT(E60, ", ", F60))</f>
-        <v>54, 57</v>
+        <f t="shared" si="24"/>
+        <v>57, 59</v>
       </c>
       <c r="H60" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="I60" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61">
-        <v>58</v>
-      </c>
-      <c r="D61">
-        <v>59</v>
-      </c>
-      <c r="E61">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G61" s="8"/>
+    </row>
+    <row r="63" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B63" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+      <c r="E65">
+        <f>C65-1</f>
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <f>D65</f>
+        <v>4</v>
+      </c>
+      <c r="G65" s="5" t="str">
+        <f t="shared" ref="G65:G72" si="25">IF(D65 = 0, E65, _xlfn.CONCAT(E65, ", ", F65))</f>
+        <v>2, 4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" t="s">
+        <v>10</v>
+      </c>
+      <c r="J65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>13</v>
+      </c>
+      <c r="E66">
+        <f>C66-1</f>
+        <v>4</v>
+      </c>
+      <c r="F66">
+        <f>D66</f>
+        <v>13</v>
+      </c>
+      <c r="G66" s="5" t="str">
         <f t="shared" si="25"/>
-        <v>57</v>
-      </c>
-      <c r="F61">
+        <v>4, 13</v>
+      </c>
+      <c r="I66" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>25</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E72" si="26">C67-1</f>
+        <v>13</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F72" si="27">D67</f>
+        <v>25</v>
+      </c>
+      <c r="G67" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>13, 25</v>
+      </c>
+      <c r="I67" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68">
+        <v>26</v>
+      </c>
+      <c r="D68">
+        <v>29</v>
+      </c>
+      <c r="E68">
         <f t="shared" si="26"/>
-        <v>59</v>
-      </c>
-      <c r="G61" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="F68">
         <f t="shared" si="27"/>
-        <v>57, 59</v>
-      </c>
-      <c r="H61" t="s">
-        <v>79</v>
-      </c>
-      <c r="I61" t="s">
-        <v>80</v>
-      </c>
-      <c r="J61" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B62" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62">
-        <v>58</v>
-      </c>
-      <c r="D62">
-        <v>59</v>
-      </c>
-      <c r="E62">
+        <v>29</v>
+      </c>
+      <c r="G68" s="5" t="str">
         <f t="shared" si="25"/>
-        <v>57</v>
-      </c>
-      <c r="F62">
+        <v>25, 29</v>
+      </c>
+      <c r="I68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J68" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69">
+        <v>30</v>
+      </c>
+      <c r="D69">
+        <v>31</v>
+      </c>
+      <c r="E69">
         <f t="shared" si="26"/>
-        <v>59</v>
-      </c>
-      <c r="G62" s="7" t="str">
+        <v>29</v>
+      </c>
+      <c r="F69">
         <f t="shared" si="27"/>
-        <v>57, 59</v>
-      </c>
-      <c r="H62" t="s">
-        <v>79</v>
-      </c>
-      <c r="I62" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>29, 31</v>
+      </c>
+      <c r="I69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70">
+        <v>32</v>
+      </c>
+      <c r="D70">
+        <v>33</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="26"/>
+        <v>31</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="27"/>
+        <v>33</v>
+      </c>
+      <c r="G70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>31, 33</v>
+      </c>
+      <c r="I70" t="s">
+        <v>50</v>
+      </c>
+      <c r="J70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
         <v>82</v>
       </c>
-      <c r="J62" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G63" s="8"/>
-    </row>
-    <row r="65" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B65" s="2" t="s">
+      <c r="C71">
+        <v>34</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="26"/>
+        <v>33</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="5">
+        <f t="shared" si="25"/>
+        <v>33</v>
+      </c>
+      <c r="H71" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B66" s="1" t="s">
+      <c r="I71" t="s">
+        <v>83</v>
+      </c>
+      <c r="J71" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72">
+        <v>35</v>
+      </c>
+      <c r="D72">
+        <v>36</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="26"/>
+        <v>34</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="27"/>
+        <v>36</v>
+      </c>
+      <c r="G72" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>34, 36</v>
+      </c>
+      <c r="H72" t="s">
+        <v>86</v>
+      </c>
+      <c r="I72" t="s">
+        <v>85</v>
+      </c>
+      <c r="J72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B76" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="I76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" t="s">
         <v>37</v>
       </c>
-      <c r="C67">
+      <c r="C77">
         <v>3</v>
       </c>
-      <c r="D67">
+      <c r="D77">
         <v>4</v>
       </c>
-      <c r="E67">
-        <f>C67-1</f>
+      <c r="E77">
+        <f>C77-1</f>
         <v>2</v>
       </c>
-      <c r="F67">
-        <f>D67</f>
+      <c r="F77">
+        <f>D77</f>
         <v>4</v>
       </c>
-      <c r="G67" s="5" t="str">
-        <f t="shared" ref="G67:G74" si="28">IF(D67 = 0, E67, _xlfn.CONCAT(E67, ", ", F67))</f>
+      <c r="G77" s="7" t="str">
+        <f t="shared" ref="G77:G91" si="28">IF(D77 = 0, E77, _xlfn.CONCAT(E77, ", ", F77))</f>
         <v>2, 4</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H77" t="s">
         <v>9</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I77" t="s">
         <v>10</v>
       </c>
-      <c r="J67" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
+      <c r="J77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" t="s">
         <v>11</v>
       </c>
-      <c r="C68">
+      <c r="C78">
         <v>5</v>
       </c>
-      <c r="D68">
+      <c r="D78">
         <v>13</v>
       </c>
-      <c r="E68">
-        <f>C68-1</f>
+      <c r="E78">
+        <f>C78-1</f>
         <v>4</v>
       </c>
-      <c r="F68">
-        <f>D68</f>
+      <c r="F78">
+        <f>D78</f>
         <v>13</v>
       </c>
-      <c r="G68" s="5" t="str">
+      <c r="G78" s="7" t="str">
         <f t="shared" si="28"/>
         <v>4, 13</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I78" t="s">
         <v>12</v>
       </c>
-      <c r="J68" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
+      <c r="J78" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" t="s">
         <v>13</v>
       </c>
-      <c r="C69">
+      <c r="C79">
         <v>14</v>
       </c>
-      <c r="D69">
+      <c r="D79">
         <v>25</v>
       </c>
-      <c r="E69">
-        <f t="shared" ref="E69:E74" si="29">C69-1</f>
+      <c r="E79">
+        <f t="shared" ref="E79:E91" si="29">C79-1</f>
         <v>13</v>
       </c>
-      <c r="F69">
-        <f t="shared" ref="F69:F74" si="30">D69</f>
+      <c r="F79">
+        <f t="shared" ref="F79:F91" si="30">D79</f>
         <v>25</v>
       </c>
-      <c r="G69" s="5" t="str">
+      <c r="G79" s="7" t="str">
         <f t="shared" si="28"/>
         <v>13, 25</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I79" t="s">
         <v>14</v>
       </c>
-      <c r="J69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
+      <c r="J79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" t="s">
         <v>45</v>
       </c>
-      <c r="C70">
+      <c r="C80">
         <v>26</v>
       </c>
-      <c r="D70">
+      <c r="D80">
         <v>29</v>
       </c>
-      <c r="E70">
+      <c r="E80">
         <f t="shared" si="29"/>
         <v>25</v>
       </c>
-      <c r="F70">
+      <c r="F80">
         <f t="shared" si="30"/>
         <v>29</v>
       </c>
-      <c r="G70" s="5" t="str">
+      <c r="G80" s="7" t="str">
         <f t="shared" si="28"/>
         <v>25, 29</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I80" t="s">
         <v>46</v>
       </c>
-      <c r="J70" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+      <c r="J80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" t="s">
         <v>45</v>
       </c>
-      <c r="C71">
+      <c r="C81">
         <v>30</v>
       </c>
-      <c r="D71">
+      <c r="D81">
         <v>31</v>
       </c>
-      <c r="E71">
+      <c r="E81">
         <f t="shared" si="29"/>
         <v>29</v>
       </c>
-      <c r="F71">
+      <c r="F81">
         <f t="shared" si="30"/>
         <v>31</v>
       </c>
-      <c r="G71" s="5" t="str">
+      <c r="G81" s="7" t="str">
         <f t="shared" si="28"/>
         <v>29, 31</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I81" t="s">
         <v>47</v>
       </c>
-      <c r="J71" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
+      <c r="J81" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" t="s">
         <v>45</v>
       </c>
-      <c r="C72">
+      <c r="C82">
         <v>32</v>
       </c>
-      <c r="D72">
+      <c r="D82">
         <v>33</v>
       </c>
-      <c r="E72">
+      <c r="E82">
         <f t="shared" si="29"/>
         <v>31</v>
       </c>
-      <c r="F72">
+      <c r="F82">
         <f t="shared" si="30"/>
         <v>33</v>
       </c>
-      <c r="G72" s="5" t="str">
+      <c r="G82" s="7" t="str">
         <f t="shared" si="28"/>
         <v>31, 33</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I82" t="s">
         <v>50</v>
       </c>
-      <c r="J72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73">
+      <c r="J82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+      <c r="C83">
         <v>34</v>
       </c>
-      <c r="E73">
+      <c r="D83">
+        <v>36</v>
+      </c>
+      <c r="E83">
         <f t="shared" si="29"/>
         <v>33</v>
       </c>
-      <c r="F73">
+      <c r="F83">
+        <f t="shared" si="30"/>
+        <v>36</v>
+      </c>
+      <c r="G83" s="7" t="str">
+        <f t="shared" si="28"/>
+        <v>33, 36</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I83" t="s">
+        <v>90</v>
+      </c>
+      <c r="J83" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>126</v>
+      </c>
+      <c r="B84" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84">
+        <v>37</v>
+      </c>
+      <c r="D84">
+        <v>39</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="29"/>
+        <v>36</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="30"/>
+        <v>39</v>
+      </c>
+      <c r="G84" s="7" t="str">
+        <f t="shared" si="28"/>
+        <v>36, 39</v>
+      </c>
+      <c r="H84" t="s">
+        <v>63</v>
+      </c>
+      <c r="I84" t="s">
+        <v>64</v>
+      </c>
+      <c r="J84" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85">
+        <v>67</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="29"/>
+        <v>66</v>
+      </c>
+      <c r="F85">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="G73" s="5">
+      <c r="G85" s="7">
         <f t="shared" si="28"/>
-        <v>33</v>
-      </c>
-      <c r="H73" t="s">
-        <v>85</v>
-      </c>
-      <c r="I73" t="s">
-        <v>85</v>
-      </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
-        <v>86</v>
-      </c>
-      <c r="C74">
-        <v>35</v>
-      </c>
-      <c r="D74">
-        <v>36</v>
-      </c>
-      <c r="E74">
+        <v>66</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I85" t="s">
+        <v>91</v>
+      </c>
+      <c r="J85" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86">
+        <v>68</v>
+      </c>
+      <c r="D86">
+        <v>69</v>
+      </c>
+      <c r="E86">
         <f t="shared" si="29"/>
-        <v>34</v>
-      </c>
-      <c r="F74">
+        <v>67</v>
+      </c>
+      <c r="F86">
         <f t="shared" si="30"/>
-        <v>36</v>
-      </c>
-      <c r="G74" s="5" t="str">
+        <v>69</v>
+      </c>
+      <c r="G86" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>34, 36</v>
-      </c>
-      <c r="H74" t="s">
-        <v>88</v>
-      </c>
-      <c r="I74" t="s">
-        <v>87</v>
-      </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G75" s="5"/>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G76" s="5"/>
-    </row>
-    <row r="77" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B77" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B78" s="1" t="s">
+        <v>67, 69</v>
+      </c>
+      <c r="H86" t="s">
+        <v>94</v>
+      </c>
+      <c r="I86" t="s">
+        <v>94</v>
+      </c>
+      <c r="J86" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87">
+        <v>70</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="29"/>
+        <v>69</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G87" s="7">
+        <f t="shared" si="28"/>
+        <v>69</v>
+      </c>
+      <c r="H87" t="s">
+        <v>96</v>
+      </c>
+      <c r="I87" t="s">
+        <v>96</v>
+      </c>
+      <c r="J87" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B88" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88">
+        <v>71</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="29"/>
+        <v>70</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G88" s="7">
+        <f t="shared" si="28"/>
+        <v>70</v>
+      </c>
+      <c r="H88" t="s">
+        <v>97</v>
+      </c>
+      <c r="I88" t="s">
+        <v>97</v>
+      </c>
+      <c r="J88" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>126</v>
+      </c>
+      <c r="B89" t="s">
+        <v>98</v>
+      </c>
+      <c r="C89">
+        <v>72</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="29"/>
+        <v>71</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="G89" s="7">
+        <f t="shared" si="28"/>
+        <v>71</v>
+      </c>
+      <c r="H89" t="s">
+        <v>97</v>
+      </c>
+      <c r="I89" t="s">
+        <v>98</v>
+      </c>
+      <c r="J89" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>126</v>
+      </c>
+      <c r="B90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90">
+        <v>74</v>
+      </c>
+      <c r="D90">
+        <v>75</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="29"/>
+        <v>73</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="G90" s="7" t="str">
+        <f t="shared" si="28"/>
+        <v>73, 75</v>
+      </c>
+      <c r="H90" t="s">
+        <v>100</v>
+      </c>
+      <c r="I90" t="s">
+        <v>102</v>
+      </c>
+      <c r="J90" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" t="s">
+        <v>103</v>
+      </c>
+      <c r="C91">
+        <v>74</v>
+      </c>
+      <c r="D91">
+        <v>75</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="29"/>
+        <v>73</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="30"/>
+        <v>75</v>
+      </c>
+      <c r="G91" s="7" t="str">
+        <f t="shared" si="28"/>
+        <v>73, 75</v>
+      </c>
+      <c r="H91" t="s">
+        <v>101</v>
+      </c>
+      <c r="I91" t="s">
+        <v>101</v>
+      </c>
+      <c r="J91" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B93" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B94" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="G94" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H94" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I78" s="1" t="s">
+      <c r="I94" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="J94" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" t="s">
         <v>37</v>
       </c>
-      <c r="C79">
+      <c r="C95">
         <v>3</v>
       </c>
-      <c r="D79">
+      <c r="D95">
         <v>4</v>
       </c>
-      <c r="E79">
-        <f>C79-1</f>
+      <c r="E95">
+        <f>C95-1</f>
         <v>2</v>
       </c>
-      <c r="F79">
-        <f>D79</f>
+      <c r="F95">
+        <f>D95</f>
         <v>4</v>
       </c>
-      <c r="G79" s="5" t="str">
-        <f t="shared" ref="G79:G93" si="31">IF(D79 = 0, E79, _xlfn.CONCAT(E79, ", ", F79))</f>
+      <c r="G95" s="7" t="str">
+        <f t="shared" ref="G95:G104" si="31">IF(D95 = 0, E95, _xlfn.CONCAT(E95, ", ", F95))</f>
         <v>2, 4</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H95" t="s">
         <v>9</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I95" t="s">
         <v>10</v>
       </c>
-      <c r="J79" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B80" t="s">
+      <c r="J95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96" t="s">
         <v>11</v>
       </c>
-      <c r="C80">
+      <c r="C96">
         <v>5</v>
       </c>
-      <c r="D80">
+      <c r="D96">
         <v>13</v>
       </c>
-      <c r="E80">
-        <f>C80-1</f>
+      <c r="E96">
+        <f>C96-1</f>
         <v>4</v>
       </c>
-      <c r="F80">
-        <f>D80</f>
+      <c r="F96">
+        <f>D96</f>
         <v>13</v>
       </c>
-      <c r="G80" s="5" t="str">
+      <c r="G96" s="7" t="str">
         <f t="shared" si="31"/>
         <v>4, 13</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I96" t="s">
         <v>12</v>
       </c>
-      <c r="J80" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
+      <c r="J96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" t="s">
         <v>13</v>
       </c>
-      <c r="C81">
+      <c r="C97">
         <v>14</v>
       </c>
-      <c r="D81">
+      <c r="D97">
         <v>25</v>
       </c>
-      <c r="E81">
-        <f t="shared" ref="E81:E93" si="32">C81-1</f>
+      <c r="E97">
+        <f t="shared" ref="E97:E104" si="32">C97-1</f>
         <v>13</v>
       </c>
-      <c r="F81">
-        <f t="shared" ref="F81:F93" si="33">D81</f>
+      <c r="F97">
+        <f t="shared" ref="F97:F104" si="33">D97</f>
         <v>25</v>
       </c>
-      <c r="G81" s="5" t="str">
+      <c r="G97" s="7" t="str">
         <f t="shared" si="31"/>
         <v>13, 25</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I97" t="s">
         <v>14</v>
       </c>
-      <c r="J81" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
+      <c r="J97" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" t="s">
         <v>45</v>
       </c>
-      <c r="C82">
+      <c r="C98">
         <v>26</v>
       </c>
-      <c r="D82">
+      <c r="D98">
         <v>29</v>
       </c>
-      <c r="E82">
+      <c r="E98">
         <f t="shared" si="32"/>
         <v>25</v>
       </c>
-      <c r="F82">
+      <c r="F98">
         <f t="shared" si="33"/>
         <v>29</v>
       </c>
-      <c r="G82" s="5" t="str">
+      <c r="G98" s="7" t="str">
         <f t="shared" si="31"/>
         <v>25, 29</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I98" t="s">
         <v>46</v>
       </c>
-      <c r="J82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
+      <c r="J98" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>126</v>
+      </c>
+      <c r="B99" t="s">
         <v>45</v>
       </c>
-      <c r="C83">
+      <c r="C99">
         <v>30</v>
       </c>
-      <c r="D83">
+      <c r="D99">
         <v>31</v>
       </c>
-      <c r="E83">
+      <c r="E99">
         <f t="shared" si="32"/>
         <v>29</v>
       </c>
-      <c r="F83">
+      <c r="F99">
         <f t="shared" si="33"/>
         <v>31</v>
       </c>
-      <c r="G83" s="5" t="str">
+      <c r="G99" s="7" t="str">
         <f t="shared" si="31"/>
         <v>29, 31</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I99" t="s">
         <v>47</v>
       </c>
-      <c r="J83" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
+      <c r="J99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>126</v>
+      </c>
+      <c r="B100" t="s">
         <v>45</v>
       </c>
-      <c r="C84">
+      <c r="C100">
         <v>32</v>
       </c>
-      <c r="D84">
+      <c r="D100">
         <v>33</v>
       </c>
-      <c r="E84">
+      <c r="E100">
         <f t="shared" si="32"/>
         <v>31</v>
       </c>
-      <c r="F84">
+      <c r="F100">
         <f t="shared" si="33"/>
         <v>33</v>
       </c>
-      <c r="G84" s="5" t="str">
+      <c r="G100" s="7" t="str">
         <f t="shared" si="31"/>
         <v>31, 33</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I100" t="s">
         <v>50</v>
       </c>
-      <c r="J84" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B85" t="s">
-        <v>90</v>
-      </c>
-      <c r="C85">
+      <c r="J100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C101">
         <v>34</v>
       </c>
-      <c r="D85">
-        <v>36</v>
-      </c>
-      <c r="E85">
+      <c r="D101">
+        <v>35</v>
+      </c>
+      <c r="E101">
         <f t="shared" si="32"/>
         <v>33</v>
       </c>
-      <c r="F85">
+      <c r="F101">
         <f t="shared" si="33"/>
+        <v>35</v>
+      </c>
+      <c r="G101" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>33, 35</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I101" t="s">
+        <v>94</v>
+      </c>
+      <c r="J101" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>126</v>
+      </c>
+      <c r="B102" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102">
         <v>36</v>
       </c>
-      <c r="G85" s="5" t="str">
+      <c r="D102">
+        <v>37</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="32"/>
+        <v>35</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="33"/>
+        <v>37</v>
+      </c>
+      <c r="G102" s="7" t="str">
         <f t="shared" si="31"/>
-        <v>33, 36</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I85" t="s">
-        <v>92</v>
-      </c>
-      <c r="J85" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B86" t="s">
-        <v>62</v>
-      </c>
-      <c r="C86">
+        <v>35, 37</v>
+      </c>
+      <c r="H102" t="s">
+        <v>94</v>
+      </c>
+      <c r="I102" t="s">
+        <v>64</v>
+      </c>
+      <c r="J102" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103" t="s">
+        <v>96</v>
+      </c>
+      <c r="C103">
+        <v>38</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="32"/>
         <v>37</v>
       </c>
-      <c r="D86">
-        <v>39</v>
-      </c>
-      <c r="E86">
-        <f t="shared" si="32"/>
-        <v>36</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="33"/>
-        <v>39</v>
-      </c>
-      <c r="G86" s="5" t="str">
-        <f t="shared" si="31"/>
-        <v>36, 39</v>
-      </c>
-      <c r="H86" t="s">
-        <v>63</v>
-      </c>
-      <c r="I86" t="s">
-        <v>64</v>
-      </c>
-      <c r="J86" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
-        <v>94</v>
-      </c>
-      <c r="C87">
-        <v>67</v>
-      </c>
-      <c r="E87">
-        <f t="shared" si="32"/>
-        <v>66</v>
-      </c>
-      <c r="F87">
+      <c r="F103">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G87" s="5">
+      <c r="G103" s="7">
         <f t="shared" si="31"/>
-        <v>66</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I87" t="s">
-        <v>93</v>
-      </c>
-      <c r="J87" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B88" t="s">
-        <v>95</v>
-      </c>
-      <c r="C88">
-        <v>68</v>
-      </c>
-      <c r="D88">
-        <v>69</v>
-      </c>
-      <c r="E88">
+        <v>37</v>
+      </c>
+      <c r="H103" t="s">
+        <v>96</v>
+      </c>
+      <c r="I103" t="s">
+        <v>96</v>
+      </c>
+      <c r="J103" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+      <c r="B104" t="s">
+        <v>97</v>
+      </c>
+      <c r="C104">
+        <v>39</v>
+      </c>
+      <c r="E104">
         <f t="shared" si="32"/>
-        <v>67</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="33"/>
-        <v>69</v>
-      </c>
-      <c r="G88" s="5" t="str">
-        <f t="shared" si="31"/>
-        <v>67, 69</v>
-      </c>
-      <c r="H88" t="s">
-        <v>96</v>
-      </c>
-      <c r="I88" t="s">
-        <v>96</v>
-      </c>
-      <c r="J88" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89">
-        <v>70</v>
-      </c>
-      <c r="E89">
-        <f t="shared" si="32"/>
-        <v>69</v>
-      </c>
-      <c r="F89">
+        <v>38</v>
+      </c>
+      <c r="F104">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="G89" s="5">
+      <c r="G104" s="7">
         <f t="shared" si="31"/>
-        <v>69</v>
-      </c>
-      <c r="H89" t="s">
-        <v>98</v>
-      </c>
-      <c r="I89" t="s">
-        <v>98</v>
-      </c>
-      <c r="J89" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90">
-        <v>71</v>
-      </c>
-      <c r="E90">
-        <f t="shared" si="32"/>
-        <v>70</v>
-      </c>
-      <c r="F90">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="G90" s="5">
-        <f t="shared" si="31"/>
-        <v>70</v>
-      </c>
-      <c r="H90" t="s">
-        <v>99</v>
-      </c>
-      <c r="I90" t="s">
-        <v>99</v>
-      </c>
-      <c r="J90" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>100</v>
-      </c>
-      <c r="C91">
-        <v>72</v>
-      </c>
-      <c r="E91">
-        <f t="shared" si="32"/>
-        <v>71</v>
-      </c>
-      <c r="F91">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="5">
-        <f t="shared" si="31"/>
-        <v>71</v>
-      </c>
-      <c r="H91" t="s">
-        <v>99</v>
-      </c>
-      <c r="I91" t="s">
-        <v>100</v>
-      </c>
-      <c r="J91" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>101</v>
-      </c>
-      <c r="C92">
-        <v>74</v>
-      </c>
-      <c r="D92">
-        <v>75</v>
-      </c>
-      <c r="E92">
-        <f t="shared" si="32"/>
-        <v>73</v>
-      </c>
-      <c r="F92">
-        <f t="shared" si="33"/>
-        <v>75</v>
-      </c>
-      <c r="G92" s="5" t="str">
-        <f t="shared" si="31"/>
-        <v>73, 75</v>
-      </c>
-      <c r="H92" t="s">
-        <v>102</v>
-      </c>
-      <c r="I92" t="s">
-        <v>104</v>
-      </c>
-      <c r="J92" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
-        <v>105</v>
-      </c>
-      <c r="C93">
-        <v>74</v>
-      </c>
-      <c r="D93">
-        <v>75</v>
-      </c>
-      <c r="E93">
-        <f t="shared" si="32"/>
-        <v>73</v>
-      </c>
-      <c r="F93">
-        <f t="shared" si="33"/>
-        <v>75</v>
-      </c>
-      <c r="G93" s="5" t="str">
-        <f t="shared" si="31"/>
-        <v>73, 75</v>
-      </c>
-      <c r="H93" t="s">
-        <v>103</v>
-      </c>
-      <c r="I93" t="s">
-        <v>103</v>
-      </c>
-      <c r="J93" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G94" s="5"/>
-    </row>
-    <row r="95" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B95" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B96" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H104" t="s">
+        <v>97</v>
+      </c>
+      <c r="I104" t="s">
+        <v>97</v>
+      </c>
+      <c r="J104" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G105" s="8"/>
+    </row>
+    <row r="107" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B107" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B108" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F108" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G96" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H108" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I96" s="1" t="s">
+      <c r="I108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J96" s="1" t="s">
+      <c r="J108" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
         <v>37</v>
       </c>
-      <c r="C97">
+      <c r="C109">
         <v>3</v>
       </c>
-      <c r="D97">
+      <c r="D109">
         <v>4</v>
       </c>
-      <c r="E97">
-        <f>C97-1</f>
+      <c r="E109">
+        <f>C109-1</f>
         <v>2</v>
       </c>
-      <c r="F97">
-        <f>D97</f>
+      <c r="F109">
+        <f>D109</f>
         <v>4</v>
       </c>
-      <c r="G97" s="5" t="str">
-        <f t="shared" ref="G97:G106" si="34">IF(D97 = 0, E97, _xlfn.CONCAT(E97, ", ", F97))</f>
+      <c r="G109" s="5" t="str">
+        <f t="shared" ref="G109:G123" si="34">IF(D109 = 0, E109, _xlfn.CONCAT(E109, ", ", F109))</f>
         <v>2, 4</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H109" t="s">
         <v>9</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I109" t="s">
         <v>10</v>
       </c>
-      <c r="J97" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B98" t="s">
+      <c r="J109" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
         <v>11</v>
       </c>
-      <c r="C98">
+      <c r="C110">
         <v>5</v>
       </c>
-      <c r="D98">
+      <c r="D110">
         <v>13</v>
       </c>
-      <c r="E98">
-        <f>C98-1</f>
+      <c r="E110">
+        <f>C110-1</f>
         <v>4</v>
       </c>
-      <c r="F98">
-        <f>D98</f>
+      <c r="F110">
+        <f>D110</f>
         <v>13</v>
       </c>
-      <c r="G98" s="5" t="str">
+      <c r="G110" s="5" t="str">
         <f t="shared" si="34"/>
         <v>4, 13</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I110" t="s">
         <v>12</v>
       </c>
-      <c r="J98" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B99" t="s">
+      <c r="J110" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
         <v>13</v>
       </c>
-      <c r="C99">
+      <c r="C111">
         <v>14</v>
       </c>
-      <c r="D99">
+      <c r="D111">
         <v>25</v>
       </c>
-      <c r="E99">
-        <f t="shared" ref="E99:E106" si="35">C99-1</f>
+      <c r="E111">
+        <f t="shared" ref="E111:E122" si="35">C111-1</f>
         <v>13</v>
       </c>
-      <c r="F99">
-        <f t="shared" ref="F99:F106" si="36">D99</f>
+      <c r="F111">
+        <f t="shared" ref="F111:F122" si="36">D111</f>
         <v>25</v>
       </c>
-      <c r="G99" s="5" t="str">
+      <c r="G111" s="5" t="str">
         <f t="shared" si="34"/>
         <v>13, 25</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I111" t="s">
         <v>14</v>
       </c>
-      <c r="J99" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B100" t="s">
-        <v>45</v>
-      </c>
-      <c r="C100">
-        <v>26</v>
-      </c>
-      <c r="D100">
-        <v>29</v>
-      </c>
-      <c r="E100">
+      <c r="J111" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>112</v>
+      </c>
+      <c r="C112">
+        <v>48</v>
+      </c>
+      <c r="D112">
+        <v>51</v>
+      </c>
+      <c r="E112">
         <f t="shared" si="35"/>
-        <v>25</v>
-      </c>
-      <c r="F100">
+        <v>47</v>
+      </c>
+      <c r="F112">
         <f t="shared" si="36"/>
-        <v>29</v>
-      </c>
-      <c r="G100" s="5" t="str">
+        <v>51</v>
+      </c>
+      <c r="G112" s="5" t="str">
         <f t="shared" si="34"/>
-        <v>25, 29</v>
-      </c>
-      <c r="I100" t="s">
+        <v>47, 51</v>
+      </c>
+      <c r="I112" t="s">
         <v>46</v>
       </c>
-      <c r="J100" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
-        <v>45</v>
-      </c>
-      <c r="C101">
-        <v>30</v>
-      </c>
-      <c r="D101">
-        <v>31</v>
-      </c>
-      <c r="E101">
+      <c r="J112" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113">
+        <v>52</v>
+      </c>
+      <c r="D113">
+        <v>53</v>
+      </c>
+      <c r="E113">
         <f t="shared" si="35"/>
-        <v>29</v>
-      </c>
-      <c r="F101">
+        <v>51</v>
+      </c>
+      <c r="F113">
         <f t="shared" si="36"/>
-        <v>31</v>
-      </c>
-      <c r="G101" s="5" t="str">
+        <v>53</v>
+      </c>
+      <c r="G113" s="5" t="str">
         <f t="shared" si="34"/>
-        <v>29, 31</v>
-      </c>
-      <c r="I101" t="s">
+        <v>51, 53</v>
+      </c>
+      <c r="I113" t="s">
         <v>47</v>
       </c>
-      <c r="J101" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B102" t="s">
-        <v>45</v>
-      </c>
-      <c r="C102">
-        <v>32</v>
-      </c>
-      <c r="D102">
-        <v>33</v>
-      </c>
-      <c r="E102">
+      <c r="J113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114">
+        <v>54</v>
+      </c>
+      <c r="D114">
+        <v>55</v>
+      </c>
+      <c r="E114">
         <f t="shared" si="35"/>
-        <v>31</v>
-      </c>
-      <c r="F102">
+        <v>53</v>
+      </c>
+      <c r="F114">
         <f t="shared" si="36"/>
-        <v>33</v>
-      </c>
-      <c r="G102" s="5" t="str">
+        <v>55</v>
+      </c>
+      <c r="G114" s="5" t="str">
         <f t="shared" si="34"/>
-        <v>31, 33</v>
-      </c>
-      <c r="I102" t="s">
+        <v>53, 55</v>
+      </c>
+      <c r="I114" t="s">
         <v>50</v>
       </c>
-      <c r="J102" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B103" t="s">
-        <v>107</v>
-      </c>
-      <c r="C103">
-        <v>34</v>
-      </c>
-      <c r="D103">
-        <v>35</v>
-      </c>
-      <c r="E103">
-        <f t="shared" si="35"/>
-        <v>33</v>
-      </c>
-      <c r="F103">
-        <f t="shared" si="36"/>
-        <v>35</v>
-      </c>
-      <c r="G103" s="5" t="str">
-        <f t="shared" si="34"/>
-        <v>33, 35</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I103" t="s">
-        <v>96</v>
-      </c>
-      <c r="J103" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B104" t="s">
+      <c r="J114" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
         <v>109</v>
       </c>
-      <c r="C104">
+      <c r="C115">
         <v>36</v>
       </c>
-      <c r="D104">
-        <v>37</v>
-      </c>
-      <c r="E104">
+      <c r="D115">
+        <v>47</v>
+      </c>
+      <c r="E115">
         <f t="shared" si="35"/>
         <v>35</v>
       </c>
-      <c r="F104">
+      <c r="F115">
         <f t="shared" si="36"/>
-        <v>37</v>
-      </c>
-      <c r="G104" s="5" t="str">
+        <v>47</v>
+      </c>
+      <c r="G115" s="5" t="str">
         <f t="shared" si="34"/>
-        <v>35, 37</v>
-      </c>
-      <c r="H104" t="s">
-        <v>96</v>
-      </c>
-      <c r="I104" t="s">
-        <v>64</v>
-      </c>
-      <c r="J104" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B105" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105">
-        <v>38</v>
-      </c>
-      <c r="E105">
-        <f t="shared" si="35"/>
-        <v>37</v>
-      </c>
-      <c r="F105">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="G105" s="5">
-        <f t="shared" si="34"/>
-        <v>37</v>
-      </c>
-      <c r="H105" t="s">
-        <v>98</v>
-      </c>
-      <c r="I105" t="s">
-        <v>98</v>
-      </c>
-      <c r="J105" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B106" t="s">
-        <v>99</v>
-      </c>
-      <c r="C106">
-        <v>39</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="35"/>
-        <v>38</v>
-      </c>
-      <c r="F106">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="G106" s="5">
-        <f t="shared" si="34"/>
-        <v>38</v>
-      </c>
-      <c r="H106" t="s">
-        <v>99</v>
-      </c>
-      <c r="I106" t="s">
-        <v>99</v>
-      </c>
-      <c r="J106" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B109" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B110" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G110" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B111" t="s">
-        <v>37</v>
-      </c>
-      <c r="C111">
-        <v>3</v>
-      </c>
-      <c r="D111">
-        <v>4</v>
-      </c>
-      <c r="E111">
-        <f>C111-1</f>
-        <v>2</v>
-      </c>
-      <c r="F111">
-        <f>D111</f>
-        <v>4</v>
-      </c>
-      <c r="G111" s="5" t="str">
-        <f t="shared" ref="G111:G125" si="37">IF(D111 = 0, E111, _xlfn.CONCAT(E111, ", ", F111))</f>
-        <v>2, 4</v>
-      </c>
-      <c r="H111" t="s">
-        <v>9</v>
-      </c>
-      <c r="I111" t="s">
-        <v>10</v>
-      </c>
-      <c r="J111" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B112" t="s">
-        <v>11</v>
-      </c>
-      <c r="C112">
-        <v>5</v>
-      </c>
-      <c r="D112">
-        <v>13</v>
-      </c>
-      <c r="E112">
-        <f>C112-1</f>
-        <v>4</v>
-      </c>
-      <c r="F112">
-        <f>D112</f>
-        <v>13</v>
-      </c>
-      <c r="G112" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>4, 13</v>
-      </c>
-      <c r="I112" t="s">
-        <v>12</v>
-      </c>
-      <c r="J112" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B113" t="s">
-        <v>13</v>
-      </c>
-      <c r="C113">
-        <v>14</v>
-      </c>
-      <c r="D113">
-        <v>25</v>
-      </c>
-      <c r="E113">
-        <f t="shared" ref="E113:E124" si="38">C113-1</f>
-        <v>13</v>
-      </c>
-      <c r="F113">
-        <f t="shared" ref="F113:F124" si="39">D113</f>
-        <v>25</v>
-      </c>
-      <c r="G113" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>13, 25</v>
-      </c>
-      <c r="I113" t="s">
-        <v>14</v>
-      </c>
-      <c r="J113" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B114" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114">
-        <v>48</v>
-      </c>
-      <c r="D114">
-        <v>51</v>
-      </c>
-      <c r="E114">
-        <f t="shared" si="38"/>
-        <v>47</v>
-      </c>
-      <c r="F114">
-        <f t="shared" si="39"/>
-        <v>51</v>
-      </c>
-      <c r="G114" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>47, 51</v>
-      </c>
-      <c r="I114" t="s">
-        <v>46</v>
-      </c>
-      <c r="J114" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B115" t="s">
-        <v>114</v>
-      </c>
-      <c r="C115">
-        <v>52</v>
-      </c>
-      <c r="D115">
-        <v>53</v>
-      </c>
-      <c r="E115">
-        <f t="shared" si="38"/>
-        <v>51</v>
-      </c>
-      <c r="F115">
-        <f t="shared" si="39"/>
-        <v>53</v>
-      </c>
-      <c r="G115" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>51, 53</v>
+        <v>35, 47</v>
       </c>
       <c r="I115" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="J115" t="s">
         <v>41</v>
@@ -3687,28 +3903,28 @@
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C116">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D116">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E116">
-        <f t="shared" si="38"/>
-        <v>53</v>
+        <f t="shared" si="35"/>
+        <v>57</v>
       </c>
       <c r="F116">
-        <f t="shared" si="39"/>
-        <v>55</v>
+        <f t="shared" si="36"/>
+        <v>60</v>
       </c>
       <c r="G116" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>53, 55</v>
+        <f t="shared" si="34"/>
+        <v>57, 60</v>
       </c>
       <c r="I116" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J116" t="s">
         <v>41</v>
@@ -3716,28 +3932,31 @@
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C117">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D117">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E117">
-        <f t="shared" si="38"/>
-        <v>35</v>
+        <f t="shared" si="35"/>
+        <v>60</v>
       </c>
       <c r="F117">
-        <f t="shared" si="39"/>
-        <v>47</v>
+        <f t="shared" si="36"/>
+        <v>62</v>
       </c>
       <c r="G117" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>35, 47</v>
+        <f t="shared" si="34"/>
+        <v>60, 62</v>
+      </c>
+      <c r="H117" t="s">
+        <v>72</v>
       </c>
       <c r="I117" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J117" t="s">
         <v>41</v>
@@ -3748,121 +3967,118 @@
         <v>115</v>
       </c>
       <c r="C118">
-        <v>58</v>
-      </c>
-      <c r="D118">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E118">
-        <f t="shared" si="38"/>
-        <v>57</v>
+        <f t="shared" si="35"/>
+        <v>62</v>
       </c>
       <c r="F118">
-        <f t="shared" si="39"/>
-        <v>60</v>
-      </c>
-      <c r="G118" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>57, 60</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="5">
+        <f t="shared" si="34"/>
+        <v>62</v>
+      </c>
+      <c r="H118" t="s">
+        <v>115</v>
       </c>
       <c r="I118" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="J118" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C119">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D119">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E119">
-        <f t="shared" si="38"/>
-        <v>60</v>
+        <f t="shared" si="35"/>
+        <v>66</v>
       </c>
       <c r="F119">
-        <f t="shared" si="39"/>
-        <v>62</v>
+        <f t="shared" si="36"/>
+        <v>68</v>
       </c>
       <c r="G119" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>60, 62</v>
+        <f t="shared" si="34"/>
+        <v>66, 68</v>
       </c>
       <c r="H119" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I119" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="J119" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C120">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E120">
-        <f t="shared" si="38"/>
-        <v>62</v>
+        <f t="shared" si="35"/>
+        <v>68</v>
       </c>
       <c r="F120">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G120" s="5">
-        <f t="shared" si="37"/>
-        <v>62</v>
+        <f t="shared" si="34"/>
+        <v>68</v>
       </c>
       <c r="H120" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="I120" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="J120" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C121">
-        <v>67</v>
-      </c>
-      <c r="D121">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E121">
-        <f t="shared" si="38"/>
-        <v>66</v>
+        <f t="shared" si="35"/>
+        <v>69</v>
       </c>
       <c r="F121">
-        <f t="shared" si="39"/>
-        <v>68</v>
-      </c>
-      <c r="G121" s="5" t="str">
-        <f t="shared" si="37"/>
-        <v>66, 68</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="5">
+        <f t="shared" si="34"/>
+        <v>69</v>
       </c>
       <c r="H121" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I121" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J121" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.35">
@@ -3870,22 +4086,22 @@
         <v>98</v>
       </c>
       <c r="C122">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E122">
-        <f t="shared" si="38"/>
-        <v>68</v>
+        <f t="shared" si="35"/>
+        <v>70</v>
       </c>
       <c r="F122">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G122" s="5">
-        <f t="shared" si="37"/>
-        <v>68</v>
+        <f t="shared" si="34"/>
+        <v>70</v>
       </c>
       <c r="H122" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I122" t="s">
         <v>98</v>
@@ -3895,130 +4111,130 @@
       </c>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B123" t="s">
-        <v>99</v>
-      </c>
-      <c r="C123">
-        <v>70</v>
-      </c>
-      <c r="E123">
-        <f t="shared" si="38"/>
-        <v>69</v>
-      </c>
-      <c r="F123">
-        <f t="shared" si="39"/>
+      <c r="G123" s="5">
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="G123" s="5">
+    </row>
+    <row r="124" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B124" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B125" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B126" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126">
+        <v>4</v>
+      </c>
+      <c r="E126">
+        <f>C126-1</f>
+        <v>2</v>
+      </c>
+      <c r="F126">
+        <f>D126</f>
+        <v>4</v>
+      </c>
+      <c r="G126" s="5" t="str">
+        <f t="shared" ref="G126:G138" si="37">IF(D126 = 0, E126, _xlfn.CONCAT(E126, ", ", F126))</f>
+        <v>2, 4</v>
+      </c>
+      <c r="H126" t="s">
+        <v>9</v>
+      </c>
+      <c r="I126" t="s">
+        <v>10</v>
+      </c>
+      <c r="J126" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B127" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127">
+        <v>5</v>
+      </c>
+      <c r="D127">
+        <v>13</v>
+      </c>
+      <c r="E127">
+        <f>C127-1</f>
+        <v>4</v>
+      </c>
+      <c r="F127">
+        <f>D127</f>
+        <v>13</v>
+      </c>
+      <c r="G127" s="5" t="str">
         <f t="shared" si="37"/>
-        <v>69</v>
-      </c>
-      <c r="H123" t="s">
-        <v>99</v>
-      </c>
-      <c r="I123" t="s">
-        <v>99</v>
-      </c>
-      <c r="J123" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B124" t="s">
-        <v>100</v>
-      </c>
-      <c r="C124">
-        <v>71</v>
-      </c>
-      <c r="E124">
-        <f t="shared" si="38"/>
-        <v>70</v>
-      </c>
-      <c r="F124">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="G124" s="5">
-        <f t="shared" si="37"/>
-        <v>70</v>
-      </c>
-      <c r="H124" t="s">
-        <v>99</v>
-      </c>
-      <c r="I124" t="s">
-        <v>100</v>
-      </c>
-      <c r="J124" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G125" s="5">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B126" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B127" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G127" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I127" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J127" s="1" t="s">
-        <v>39</v>
+        <v>4, 13</v>
+      </c>
+      <c r="I127" t="s">
+        <v>12</v>
+      </c>
+      <c r="J127" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="C128">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D128">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E128">
-        <f>C128-1</f>
-        <v>2</v>
+        <f t="shared" ref="E128" si="38">C128-1</f>
+        <v>13</v>
       </c>
       <c r="F128">
-        <f>D128</f>
-        <v>4</v>
+        <f t="shared" ref="F128" si="39">D128</f>
+        <v>25</v>
       </c>
       <c r="G128" s="5" t="str">
-        <f t="shared" ref="G128:G140" si="40">IF(D128 = 0, E128, _xlfn.CONCAT(E128, ", ", F128))</f>
-        <v>2, 4</v>
-      </c>
-      <c r="H128" t="s">
-        <v>9</v>
+        <f t="shared" si="37"/>
+        <v>13, 25</v>
       </c>
       <c r="I128" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="J128" t="s">
         <v>41</v>
@@ -4026,28 +4242,28 @@
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C129">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D129">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E129">
-        <f>C129-1</f>
-        <v>4</v>
+        <f t="shared" ref="E129:E138" si="40">C129-1</f>
+        <v>25</v>
       </c>
       <c r="F129">
-        <f>D129</f>
-        <v>13</v>
+        <f t="shared" ref="F129:F138" si="41">D129</f>
+        <v>29</v>
       </c>
       <c r="G129" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>4, 13</v>
+        <f t="shared" si="37"/>
+        <v>25, 29</v>
       </c>
       <c r="I129" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="J129" t="s">
         <v>41</v>
@@ -4055,28 +4271,28 @@
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C130">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D130">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E130">
-        <f t="shared" ref="E130" si="41">C130-1</f>
-        <v>13</v>
+        <f t="shared" si="40"/>
+        <v>29</v>
       </c>
       <c r="F130">
-        <f t="shared" ref="F130" si="42">D130</f>
-        <v>25</v>
+        <f t="shared" si="41"/>
+        <v>31</v>
       </c>
       <c r="G130" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>13, 25</v>
+        <f t="shared" si="37"/>
+        <v>29, 31</v>
       </c>
       <c r="I130" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="J130" t="s">
         <v>41</v>
@@ -4084,28 +4300,28 @@
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C131">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D131">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E140" si="43">C131-1</f>
-        <v>25</v>
+        <f t="shared" si="40"/>
+        <v>31</v>
       </c>
       <c r="F131">
-        <f t="shared" ref="F131:F140" si="44">D131</f>
-        <v>29</v>
+        <f t="shared" si="41"/>
+        <v>33</v>
       </c>
       <c r="G131" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>25, 29</v>
+        <f t="shared" si="37"/>
+        <v>31, 33</v>
       </c>
       <c r="I131" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J131" t="s">
         <v>41</v>
@@ -4113,28 +4329,31 @@
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C132">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D132">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E132">
-        <f t="shared" si="43"/>
-        <v>29</v>
+        <f t="shared" si="40"/>
+        <v>40</v>
       </c>
       <c r="F132">
-        <f t="shared" si="44"/>
-        <v>31</v>
+        <f t="shared" si="41"/>
+        <v>43</v>
       </c>
       <c r="G132" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>29, 31</v>
+        <f t="shared" si="37"/>
+        <v>40, 43</v>
+      </c>
+      <c r="H132" t="s">
+        <v>66</v>
       </c>
       <c r="I132" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="J132" t="s">
         <v>41</v>
@@ -4145,25 +4364,28 @@
         <v>114</v>
       </c>
       <c r="C133">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D133">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E133">
-        <f t="shared" si="43"/>
-        <v>31</v>
+        <f t="shared" si="40"/>
+        <v>43</v>
       </c>
       <c r="F133">
-        <f t="shared" si="44"/>
-        <v>33</v>
+        <f t="shared" si="41"/>
+        <v>45</v>
       </c>
       <c r="G133" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>31, 33</v>
+        <f t="shared" si="37"/>
+        <v>43, 45</v>
+      </c>
+      <c r="H133" t="s">
+        <v>72</v>
       </c>
       <c r="I133" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J133" t="s">
         <v>41</v>
@@ -4171,127 +4393,121 @@
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C134">
-        <v>41</v>
-      </c>
-      <c r="D134">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E134">
-        <f t="shared" si="43"/>
-        <v>40</v>
+        <f>C134-1</f>
+        <v>45</v>
       </c>
       <c r="F134">
-        <f t="shared" si="44"/>
-        <v>43</v>
-      </c>
-      <c r="G134" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>40, 43</v>
+        <f>D134</f>
+        <v>0</v>
+      </c>
+      <c r="G134" s="5">
+        <f>IF(D134 = 0, E134, _xlfn.CONCAT(E134, ", ", F134))</f>
+        <v>45</v>
       </c>
       <c r="H134" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="I134" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J134" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C135">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D135">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E135">
-        <f t="shared" si="43"/>
-        <v>43</v>
+        <f t="shared" si="40"/>
+        <v>49</v>
       </c>
       <c r="F135">
-        <f t="shared" si="44"/>
-        <v>45</v>
+        <f t="shared" si="41"/>
+        <v>51</v>
       </c>
       <c r="G135" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>43, 45</v>
+        <f t="shared" si="37"/>
+        <v>49, 51</v>
       </c>
       <c r="H135" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I135" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="J135" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C136">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E136">
-        <f>C136-1</f>
-        <v>45</v>
+        <f t="shared" si="40"/>
+        <v>51</v>
       </c>
       <c r="F136">
-        <f>D136</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="G136" s="5">
-        <f>IF(D136 = 0, E136, _xlfn.CONCAT(E136, ", ", F136))</f>
-        <v>45</v>
+        <f t="shared" si="37"/>
+        <v>51</v>
       </c>
       <c r="H136" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="I136" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="J136" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C137">
-        <v>50</v>
-      </c>
-      <c r="D137">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E137">
-        <f t="shared" si="43"/>
-        <v>49</v>
+        <f t="shared" si="40"/>
+        <v>52</v>
       </c>
       <c r="F137">
-        <f t="shared" si="44"/>
-        <v>51</v>
-      </c>
-      <c r="G137" s="5" t="str">
-        <f t="shared" si="40"/>
-        <v>49, 51</v>
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="G137" s="5">
+        <f t="shared" si="37"/>
+        <v>52</v>
       </c>
       <c r="H137" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I137" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J137" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.35">
@@ -4299,85 +4515,27 @@
         <v>98</v>
       </c>
       <c r="C138">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E138">
-        <f t="shared" si="43"/>
-        <v>51</v>
+        <f t="shared" si="40"/>
+        <v>53</v>
       </c>
       <c r="F138">
-        <f t="shared" si="44"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="G138" s="5">
-        <f t="shared" si="40"/>
-        <v>51</v>
+        <f t="shared" si="37"/>
+        <v>53</v>
       </c>
       <c r="H138" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I138" t="s">
         <v>98</v>
       </c>
       <c r="J138" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="139" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B139" t="s">
-        <v>99</v>
-      </c>
-      <c r="C139">
-        <v>53</v>
-      </c>
-      <c r="E139">
-        <f t="shared" si="43"/>
-        <v>52</v>
-      </c>
-      <c r="F139">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="G139" s="5">
-        <f t="shared" si="40"/>
-        <v>52</v>
-      </c>
-      <c r="H139" t="s">
-        <v>99</v>
-      </c>
-      <c r="I139" t="s">
-        <v>99</v>
-      </c>
-      <c r="J139" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="140" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B140" t="s">
-        <v>100</v>
-      </c>
-      <c r="C140">
-        <v>54</v>
-      </c>
-      <c r="E140">
-        <f t="shared" si="43"/>
-        <v>53</v>
-      </c>
-      <c r="F140">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="G140" s="5">
-        <f t="shared" si="40"/>
-        <v>53</v>
-      </c>
-      <c r="H140" t="s">
-        <v>99</v>
-      </c>
-      <c r="I140" t="s">
-        <v>100</v>
-      </c>
-      <c r="J140" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ready for overnight run
</commit_message>
<xml_diff>
--- a/CSV plan.xlsx
+++ b/CSV plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\nibrs_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DA8F75-5A93-40AF-9015-103BAF804A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACE3DA6-FAA0-47BD-ABBA-B8C97C50575E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="2310" windowWidth="14400" windowHeight="7815" xr2:uid="{E32AB67F-C50D-4B7B-BF96-2DF95897A32B}"/>
+    <workbookView xWindow="5200" yWindow="3490" windowWidth="14400" windowHeight="7820" xr2:uid="{E32AB67F-C50D-4B7B-BF96-2DF95897A32B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4CC23E-8A46-40A2-B7BE-F33F442EEB2C}">
   <dimension ref="A2:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,22 +978,22 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D7">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>25, 29</v>
+        <v>33, 37</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>17</v>
@@ -1010,22 +1010,22 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D8">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>29, 31</v>
+        <v>37, 39</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>16</v>

</xml_diff>